<commit_message>
Validacion de medidas e ingreso de iniciativa por Especialista
</commit_message>
<xml_diff>
--- a/back-end/Web Dinamico 2/MRVMinem/Documentos/1.1 Plantilla_Etiquetado_de_eficiencia_etiquetado_congeladoras.xlsx
+++ b/back-end/Web Dinamico 2/MRVMinem/Documentos/1.1 Plantilla_Etiquetado_de_eficiencia_etiquetado_congeladoras.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22430"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22624"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Archivos Compu DELL\Escritorio\MRV MINEM 1.0 Tercer Entregable-Mantenimientos\Enfoque excel\Excel enfoque etiquetado de eficiencia energetica\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dell\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{66DEF353-2754-4720-BBAC-67679CB9AE74}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B071D922-84BC-46DA-9387-F4E5A51BA2C9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{BFB3AA29-D743-4340-AADA-08253CA88123}"/>
   </bookViews>
@@ -617,7 +617,7 @@
   <dimension ref="A1:L311"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+      <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -708,7 +708,7 @@
       </c>
       <c r="B3" s="11">
         <f t="shared" ref="B3:B66" si="0">VLOOKUP(C3,Tabla_Categoria,2,)</f>
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="C3" s="11">
         <v>8</v>
@@ -751,7 +751,7 @@
       </c>
       <c r="B4" s="11">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>9</v>
       </c>
       <c r="C4" s="11">
         <v>9</v>
@@ -794,10 +794,10 @@
       </c>
       <c r="B5" s="13">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="C5" s="13">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D5" s="13">
         <f t="shared" si="1"/>
@@ -9706,7 +9706,7 @@
       <c r="L311" s="5"/>
     </row>
   </sheetData>
-  <sheetProtection selectLockedCells="1"/>
+  <sheetProtection algorithmName="SHA-512" hashValue="sWErd8vEd9l9EX3h3Gxm+os1Qov3DP0N/iFSp2AKz7reTvlf/QCn8SdFqOGCZ63Ii6ZtiJ9BXxOW++om0+aNQA==" saltValue="0VQUuEfLxE/NJSbxbmwKuw==" spinCount="100000" sheet="1" objects="1" scenarios="1" selectLockedCells="1"/>
   <dataValidations count="7">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A3:A311" xr:uid="{325F4596-C648-4F62-A0B0-A9AA96889F86}">
       <formula1>Lista_Anno</formula1>
@@ -9741,7 +9741,7 @@
   <dimension ref="A7:P28"/>
   <sheetViews>
     <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="O21" sqref="O21"/>
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9793,7 +9793,7 @@
         <v>8</v>
       </c>
       <c r="D8" s="2">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="F8" s="4">
         <v>120</v>
@@ -9828,7 +9828,7 @@
         <v>9</v>
       </c>
       <c r="D9" s="2">
-        <v>2</v>
+        <v>9</v>
       </c>
       <c r="F9" s="4">
         <v>225</v>
@@ -9863,7 +9863,7 @@
         <v>10</v>
       </c>
       <c r="D10" s="2">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="F10" s="4">
         <v>375</v>

</xml_diff>